<commit_message>
dev: enhancement modbus, plc1200
</commit_message>
<xml_diff>
--- a/test/data/test-modbus-sheet.xlsx
+++ b/test/data/test-modbus-sheet.xlsx
@@ -44,7 +44,7 @@
     <t>slaverId</t>
   </si>
   <si>
-    <t>startAddress</t>
+    <t>address</t>
   </si>
   <si>
     <t>quality</t>
@@ -1396,7 +1396,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B60"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>

</xml_diff>